<commit_message>
refined table/ table heading
</commit_message>
<xml_diff>
--- a/manuscript/tables_figures/Table1.xlsx
+++ b/manuscript/tables_figures/Table1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kteixeira/Dropbox (Smithsonian)/GitHub/SCBI-ForestGEO/McGregor_climate-sensitivity-variation/manuscript/tables_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60116D73-BF23-024D-BD61-3C6C94CE9888}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEED99E-1607-9842-B5C2-9F90AC304FB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{CE8D29E5-35BD-D341-9E78-19425C1F1F15}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="45">
   <si>
     <t>Prediction</t>
   </si>
@@ -144,20 +144,29 @@
     <t>H3.1. Responses varied by drought</t>
   </si>
   <si>
-    <t>3.2a. Directions of responses to predictor variables is usually consistent</t>
-  </si>
-  <si>
     <t>3.2b. Set of predictor variables in best model varies across droughts</t>
   </si>
   <si>
     <t>3.1. Drought year explained variation in drought resistance</t>
+  </si>
+  <si>
+    <t>requires verification--check that it is this way in all the best models</t>
+  </si>
+  <si>
+    <t>3.2a. Directions of responses to predictor variables is consistent</t>
+  </si>
+  <si>
+    <t>my guess</t>
+  </si>
+  <si>
+    <t>(no/yes)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -192,6 +201,20 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -252,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -287,6 +310,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F2DC1C-E74B-DD44-87E0-926D1FBF2D78}">
-  <dimension ref="B1:G34"/>
+  <dimension ref="B1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -613,8 +644,7 @@
     <col min="3" max="3" width="73.33203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="6.5" customWidth="1"/>
-    <col min="7" max="7" width="5.83203125" customWidth="1"/>
+    <col min="6" max="7" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="17" thickBot="1"/>
@@ -665,39 +695,41 @@
       <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="18" t="s">
         <v>10</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="2:7">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
     </row>
     <row r="8" spans="2:7" ht="17">
       <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="18" t="s">
         <v>10</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="17">
@@ -787,7 +819,7 @@
       <c r="C19" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="18" t="s">
         <v>4</v>
       </c>
     </row>
@@ -795,7 +827,7 @@
       <c r="C20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="18" t="s">
         <v>4</v>
       </c>
     </row>
@@ -898,8 +930,8 @@
       <c r="C28" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="13" t="s">
-        <v>35</v>
+      <c r="D28" s="18" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="2:7">
@@ -909,9 +941,9 @@
     </row>
     <row r="30" spans="2:7" ht="17">
       <c r="C30" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="18" t="s">
         <v>4</v>
       </c>
     </row>
@@ -922,10 +954,10 @@
     </row>
     <row r="32" spans="2:7" ht="17">
       <c r="C32" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D32" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E32" t="s">
         <v>13</v>
@@ -940,9 +972,9 @@
     <row r="33" spans="2:7" ht="18" thickBot="1">
       <c r="B33" s="14"/>
       <c r="C33" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E33" s="14" t="s">
@@ -956,6 +988,16 @@
       </c>
     </row>
     <row r="34" spans="2:7" ht="17" thickTop="1"/>
+    <row r="35" spans="2:7" ht="17">
+      <c r="C35" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="17">
+      <c r="C36" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E3:G3"/>

</xml_diff>

<commit_message>
Added detailed info for the notes section for each prediction
</commit_message>
<xml_diff>
--- a/manuscript/tables_figures/Table1.xlsx
+++ b/manuscript/tables_figures/Table1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Smithsonian)\Github_Ian\McGregor_climate-sensitivity-variation\manuscript\tables_figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD2169D-36A2-4C1C-B7A3-421B2FA44549}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D48970-078C-4647-92F1-77F88AC3C198}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{CE8D29E5-35BD-D341-9E78-19425C1F1F15}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="96">
   <si>
     <t>Prediction</t>
   </si>
@@ -51,15 +51,6 @@
     <t>H1.3. Drought resistance is linked to rooting volume in drier microhabitats</t>
   </si>
   <si>
-    <t>(no)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes </t>
-  </si>
-  <si>
-    <t>(yes)</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -129,9 +120,6 @@
     <t>my guess</t>
   </si>
   <si>
-    <t>(no/yes)</t>
-  </si>
-  <si>
     <t>tested_traits_all</t>
   </si>
   <si>
@@ -174,9 +162,6 @@
     <t>^</t>
   </si>
   <si>
-    <t>(yes*) yes^</t>
-  </si>
-  <si>
     <t>Results</t>
   </si>
   <si>
@@ -319,6 +304,15 @@
   </si>
   <si>
     <t>this prediction should only be using top_models_dAIC</t>
+  </si>
+  <si>
+    <t>yes (tta, s); yes (tmd*, year appears in each model and has negative coefficients for each one)</t>
+  </si>
+  <si>
+    <t>yes (only two models are duplicates - 1 for 1977 scenario and 1 for 1999 scenario [resist.value~TWI.ln+rp+mean_TLP_Mpa+(1|sp)])</t>
+  </si>
+  <si>
+    <t>I believe this is answered from the other things above</t>
   </si>
 </sst>
 </file>
@@ -803,14 +797,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F2DC1C-E74B-DD44-87E0-926D1FBF2D78}">
   <dimension ref="B1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="4.625" customWidth="1"/>
-    <col min="3" max="3" width="73.375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="75.875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.375" customWidth="1"/>
     <col min="5" max="5" width="8.625" customWidth="1"/>
     <col min="6" max="7" width="8" customWidth="1"/>
@@ -826,7 +820,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
       <c r="D2" s="22" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -860,11 +854,11 @@
         <v>1999</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I4" s="4"/>
       <c r="K4" s="19" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>1</v>
@@ -879,10 +873,10 @@
         <v>1999</v>
       </c>
       <c r="P4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="Q4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:17">
@@ -892,37 +886,27 @@
     </row>
     <row r="6" spans="2:17">
       <c r="C6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
       <c r="H6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="N6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="O6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="P6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:17">
@@ -936,147 +920,116 @@
     </row>
     <row r="8" spans="2:17">
       <c r="C8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" t="s">
-        <v>34</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="M8" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="P8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q8" t="s">
         <v>78</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="O8" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="P8" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="9" spans="2:17">
       <c r="C9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="N9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="P9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="Q9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="2:17">
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:17" ht="31.5">
       <c r="C11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="H11" t="s">
+        <v>48</v>
+      </c>
+      <c r="L11" t="s">
+        <v>49</v>
+      </c>
+      <c r="M11" t="s">
+        <v>52</v>
+      </c>
+      <c r="N11" t="s">
+        <v>49</v>
+      </c>
+      <c r="O11" t="s">
         <v>53</v>
       </c>
-      <c r="L11" t="s">
-        <v>54</v>
-      </c>
-      <c r="M11" t="s">
-        <v>57</v>
-      </c>
-      <c r="N11" t="s">
-        <v>54</v>
-      </c>
-      <c r="O11" t="s">
-        <v>58</v>
-      </c>
       <c r="P11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="Q11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="2:17" ht="36" customHeight="1">
       <c r="C12" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="M12" t="s">
+        <v>66</v>
+      </c>
+      <c r="N12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O12" t="s">
         <v>71</v>
       </c>
-      <c r="N12" t="s">
-        <v>73</v>
-      </c>
-      <c r="O12" t="s">
-        <v>76</v>
-      </c>
       <c r="P12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="Q12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="2:17">
@@ -1084,511 +1037,462 @@
         <v>7</v>
       </c>
       <c r="Q13" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="2:17" ht="31.5">
       <c r="C14" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="L14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="M14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="N14" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="O14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="P14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="Q14" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="2:17">
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="2:17">
       <c r="C16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L16" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="M16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="O16" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="P16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:17">
       <c r="C17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="M17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="N17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="O17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="P17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="2:17">
       <c r="C18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="H18" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="M18" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" t="s">
-        <v>44</v>
-      </c>
-      <c r="L18" s="16" t="s">
+      <c r="N18" t="s">
+        <v>83</v>
+      </c>
+      <c r="O18" t="s">
         <v>84</v>
       </c>
-      <c r="M18" t="s">
-        <v>87</v>
-      </c>
-      <c r="N18" t="s">
-        <v>88</v>
-      </c>
-      <c r="O18" t="s">
-        <v>89</v>
-      </c>
       <c r="P18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="Q18" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="2:17" ht="31.5">
       <c r="C19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>4</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D19" s="18"/>
       <c r="H19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="M19" s="16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="N19" s="16" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="O19" s="16" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="P19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="Q19" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="2:17">
       <c r="C20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" t="s">
-        <v>49</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D20" s="16"/>
       <c r="H20" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="M20" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="N20" s="16" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="O20" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="P20" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="Q20" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="2:17">
       <c r="B21" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="2:17">
       <c r="C22" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="L22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="P22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="2:17">
       <c r="C23" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H23" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="L23" t="s">
         <v>4</v>
       </c>
       <c r="M23" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N23" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O23" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="P23" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:17">
       <c r="C24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H24" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="L24" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="P24" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="2:17" ht="31.5">
       <c r="C25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>11</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D25" s="16"/>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H25" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="P25" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="2:17">
       <c r="C26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>11</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D26" s="16"/>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="P26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="2:17">
       <c r="B27" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:17">
       <c r="C28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" t="s">
-        <v>10</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D28" s="16"/>
       <c r="H28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="L28" s="16" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="M28" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="N28" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="2:17">
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:17">
       <c r="C30" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="16"/>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" t="s">
-        <v>35</v>
-      </c>
       <c r="L30" s="16" t="s">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="M30" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N30" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O30" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="P30" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="2:17">
       <c r="B31" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="2:17">
       <c r="C32" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="E32" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G32" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H32" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L32" t="s">
-        <v>10</v>
+        <v>95</v>
       </c>
       <c r="M32" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N32" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O32" t="s">
-        <v>12</v>
-      </c>
-      <c r="P32" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="2:16" ht="16.5" thickBot="1">
       <c r="B33" s="11"/>
       <c r="C33" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>4</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D33" s="17"/>
       <c r="E33" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I33" s="3"/>
       <c r="L33" s="17" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="M33" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N33" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O33" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="P33" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="16.5" thickTop="1">
@@ -1597,26 +1501,26 @@
     </row>
     <row r="35" spans="2:16">
       <c r="C35" s="15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="2:16">
       <c r="C36" s="13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L36" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="2:16">
       <c r="D37" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L37" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated models correcting the interaction of  TWI and height
</commit_message>
<xml_diff>
--- a/manuscript/tables_figures/Table1.xlsx
+++ b/manuscript/tables_figures/Table1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Smithsonian)\Github_Ian\McGregor_climate-sensitivity-variation\manuscript\tables_figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665BEB77-EF9D-4FE4-B4C3-542EDADDDC1C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5C40C0-CA58-4E4B-B02A-9B4BCC1D8A66}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{CE8D29E5-35BD-D341-9E78-19425C1F1F15}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="94">
   <si>
     <t>Prediction</t>
   </si>
@@ -198,9 +198,6 @@
     <t>no, ns</t>
   </si>
   <si>
-    <t>yes (tta, s); yes (tmd*)</t>
-  </si>
-  <si>
     <t>*in other words, this prediction is saying height has a coefficient than dbh.</t>
   </si>
   <si>
@@ -237,27 +234,9 @@
     <t>yes (tta, ns); yes(tmd*, height only appears in 1 of 3 models, but it does have a neg. coefficient where it appears)</t>
   </si>
   <si>
-    <t>no (tta, ns); yes(tmd*, height only appears in 9 of 11 models, but it does have a neg. coefficient where it appears)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S&lt;I&lt;D&lt;C (tta, s); [tmd*: 9 of 11 models include position, S&lt;I&lt;C&lt;D for 7 of those 9, and S&lt;I&lt;D&lt;C for the remaining 2] </t>
-  </si>
-  <si>
-    <t>no (tta; ns);</t>
-  </si>
-  <si>
-    <t>yes (tta, s); yes(tmd* it is negative for the 3 models where height is independent. Where height is included as part of the interaction with TWI, height alone has a positive coefficient (0.175) even though the coefficient of the interaction itself is negative (-0.183))</t>
-  </si>
-  <si>
-    <t>yes (tta, s); yes (tmd*, the interaction appears in 1 of 4 top models)</t>
-  </si>
-  <si>
     <t>no (tta, ns); no (tmd* interaction does not appear in top models)</t>
   </si>
   <si>
-    <t>yes (tta, s); no (tmd* interaction does not appear in top models)</t>
-  </si>
-  <si>
     <t xml:space="preserve">2.1c - more diffuse porous species correlates negatively to drought resistance </t>
   </si>
   <si>
@@ -270,9 +249,6 @@
     <t>yes (tta, ns);  no (tmd*, PLA is not in any top model)</t>
   </si>
   <si>
-    <t>yes (tta, ns);  yes (tmd*, PLA appears in 5 of 11 top models, and is yes for those)</t>
-  </si>
-  <si>
     <t>yes (tta, ns), yes (tmd* rp appears in 3 of 4 top models, and is yes for those)</t>
   </si>
   <si>
@@ -291,12 +267,6 @@
     <t>yes (tta, s);  yes (tmd*, TLP appears in all top models and is yes for all of them)</t>
   </si>
   <si>
-    <t>yes (tta, ns); yes (tmd*, TLP appears in 1 of 4 top models and is yes for that one)</t>
-  </si>
-  <si>
-    <t>yes (tta, ns); yes (tmd*, TLP appears in 5 of 11 top models and is yes for those)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -313,6 +283,30 @@
   </si>
   <si>
     <t>*I believe this is answered from the other things above</t>
+  </si>
+  <si>
+    <t>yes (tta, ns); no (tmd* interaction does not appear in top models)</t>
+  </si>
+  <si>
+    <t>yes (tta, ns); yes (tmd*, TLP appears in 1 of 3 top models and is yes for that one)</t>
+  </si>
+  <si>
+    <t>yes (tta, ns);  yes (tmd*, PLA appears in 4 of 9 top models, and is yes for those)</t>
+  </si>
+  <si>
+    <t>yes (tta, ns); yes (tmd*, TLP appears in 4 of 9 top models and is yes for those)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S&lt;I&lt;D&lt;C (tta, s); [tmd*: 7 of 9 models include position, S&lt;I&lt;C&lt;D for 5 of those 7, and S&lt;I&lt;D&lt;C for the remaining 2] </t>
+  </si>
+  <si>
+    <t>no (tta, ns); yes(tmd*, height only appears in 7 of 9 models, but it does have a neg. coefficient where it appears)</t>
+  </si>
+  <si>
+    <t>yes (tta, s); yes(tmd* it is negative for all 3 models)</t>
+  </si>
+  <si>
+    <t>yes (tta, s); yes (tmd*, height is negative for all models)</t>
   </si>
 </sst>
 </file>
@@ -479,6 +473,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -488,7 +483,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F2DC1C-E74B-DD44-87E0-926D1FBF2D78}">
   <dimension ref="B1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -827,22 +821,22 @@
     <row r="2" spans="2:17" ht="16.5" thickTop="1">
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="2:17">
       <c r="B3" s="3"/>
       <c r="C3" s="7"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="2:17">
       <c r="B4" s="4"/>
@@ -936,22 +930,22 @@
         <v>40</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="P8" t="s">
         <v>40</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="2:17">
@@ -965,22 +959,22 @@
         <v>31</v>
       </c>
       <c r="L9" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" t="s">
+        <v>59</v>
+      </c>
+      <c r="N9" t="s">
         <v>61</v>
       </c>
-      <c r="M9" t="s">
-        <v>60</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>62</v>
       </c>
-      <c r="O9" t="s">
-        <v>63</v>
-      </c>
       <c r="P9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:17">
@@ -1012,7 +1006,7 @@
         <v>31</v>
       </c>
       <c r="Q11" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="2:17" ht="36" customHeight="1">
@@ -1023,22 +1017,22 @@
         <v>40</v>
       </c>
       <c r="L12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" t="s">
+        <v>65</v>
+      </c>
+      <c r="N12" t="s">
         <v>67</v>
       </c>
-      <c r="M12" t="s">
-        <v>66</v>
-      </c>
-      <c r="N12" t="s">
-        <v>68</v>
-      </c>
       <c r="O12" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="P12" t="s">
         <v>40</v>
       </c>
       <c r="Q12" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="2:17">
@@ -1046,7 +1040,7 @@
         <v>7</v>
       </c>
       <c r="Q13" s="19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="2:17" ht="31.5">
@@ -1057,22 +1051,22 @@
         <v>39</v>
       </c>
       <c r="L14" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="M14" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="N14" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="O14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="P14" t="s">
         <v>40</v>
       </c>
       <c r="Q14" s="19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="2:17">
@@ -1131,29 +1125,29 @@
     </row>
     <row r="18" spans="2:17">
       <c r="C18" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D18" s="18"/>
       <c r="H18" t="s">
         <v>40</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="M18" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="N18" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="O18" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="P18" t="s">
         <v>40</v>
       </c>
       <c r="Q18" s="19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="2:17" ht="31.5">
@@ -1165,22 +1159,22 @@
         <v>40</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="M19" s="16" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="N19" s="16" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="O19" s="16" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="P19" t="s">
         <v>40</v>
       </c>
       <c r="Q19" s="19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="2:17">
@@ -1192,13 +1186,13 @@
         <v>40</v>
       </c>
       <c r="L20" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="M20" t="s">
         <v>87</v>
       </c>
-      <c r="M20" t="s">
-        <v>88</v>
-      </c>
       <c r="N20" s="16" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="O20" t="s">
         <v>89</v>
@@ -1207,7 +1201,7 @@
         <v>40</v>
       </c>
       <c r="Q20" s="19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="2:17">
@@ -1390,14 +1384,14 @@
       <c r="H28" t="s">
         <v>36</v>
       </c>
-      <c r="L28" s="23" t="s">
-        <v>94</v>
+      <c r="L28" s="20" t="s">
+        <v>84</v>
       </c>
       <c r="M28" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="N28" s="19" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="2:17">
@@ -1423,7 +1417,7 @@
         <v>31</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="M30" t="s">
         <v>9</v>
@@ -1460,7 +1454,7 @@
         <v>35</v>
       </c>
       <c r="L32" s="19" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="M32" t="s">
         <v>9</v>
@@ -1492,7 +1486,7 @@
       </c>
       <c r="I33" s="3"/>
       <c r="L33" s="17" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="M33" s="11" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Updated Tables 1 and 3
</commit_message>
<xml_diff>
--- a/manuscript/tables_figures/Table1.xlsx
+++ b/manuscript/tables_figures/Table1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Smithsonian)\Github_Ian\McGregor_climate-sensitivity-variation\manuscript\tables_figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5C40C0-CA58-4E4B-B02A-9B4BCC1D8A66}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F009D2-71F2-432D-BAF4-926DCBC46CE9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{CE8D29E5-35BD-D341-9E78-19425C1F1F15}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="90">
   <si>
     <t>Prediction</t>
   </si>
@@ -114,12 +114,6 @@
     <t>3.1. Drought year explained variation in drought resistance</t>
   </si>
   <si>
-    <t>requires verification--check that it is this way in all the best models</t>
-  </si>
-  <si>
-    <t>my guess</t>
-  </si>
-  <si>
     <t>tested_traits_all</t>
   </si>
   <si>
@@ -154,12 +148,6 @@
   </si>
   <si>
     <t>H2.3. Size-dependent drought resistance is not driven by functional traits</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>^</t>
   </si>
   <si>
     <t>Results</t>
@@ -799,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F2DC1C-E74B-DD44-87E0-926D1FBF2D78}">
   <dimension ref="B1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -817,7 +805,10 @@
     <col min="16" max="16" width="34.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="16.5" thickBot="1"/>
+    <row r="1" spans="2:17" ht="16.5" thickBot="1">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
     <row r="2" spans="2:17" ht="16.5" thickTop="1">
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
@@ -827,6 +818,8 @@
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="2:17">
       <c r="B3" s="3"/>
@@ -856,11 +849,11 @@
         <v>1999</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I4" s="4"/>
       <c r="K4" s="19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>1</v>
@@ -875,10 +868,10 @@
         <v>1999</v>
       </c>
       <c r="P4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="Q4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:17">
@@ -893,22 +886,22 @@
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="N6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="O6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="P6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:17">
@@ -927,25 +920,25 @@
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="H8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="P8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="2:17">
@@ -956,83 +949,83 @@
         <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="M9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="O9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="2:17">
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q10" s="19"/>
     </row>
     <row r="11" spans="2:17" ht="31.5">
       <c r="C11" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H11" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" t="s">
         <v>48</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
+        <v>45</v>
+      </c>
+      <c r="O11" t="s">
         <v>49</v>
       </c>
-      <c r="M11" t="s">
-        <v>52</v>
-      </c>
-      <c r="N11" t="s">
-        <v>49</v>
-      </c>
-      <c r="O11" t="s">
-        <v>53</v>
-      </c>
       <c r="P11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q11" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="2:17" ht="36" customHeight="1">
       <c r="C12" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="M12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="O12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="P12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="Q12" s="19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:17">
@@ -1040,33 +1033,33 @@
         <v>7</v>
       </c>
       <c r="Q13" s="19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="2:17" ht="31.5">
       <c r="C14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" t="s">
+        <v>82</v>
+      </c>
+      <c r="M14" t="s">
+        <v>82</v>
+      </c>
+      <c r="N14" t="s">
+        <v>65</v>
+      </c>
+      <c r="O14" t="s">
+        <v>65</v>
+      </c>
+      <c r="P14" t="s">
         <v>38</v>
       </c>
-      <c r="H14" t="s">
-        <v>39</v>
-      </c>
-      <c r="L14" t="s">
-        <v>86</v>
-      </c>
-      <c r="M14" t="s">
-        <v>86</v>
-      </c>
-      <c r="N14" t="s">
-        <v>69</v>
-      </c>
-      <c r="O14" t="s">
-        <v>69</v>
-      </c>
-      <c r="P14" t="s">
-        <v>40</v>
-      </c>
       <c r="Q14" s="19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="2:17">
@@ -1080,22 +1073,22 @@
         <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="N16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="O16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="P16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q16" s="19"/>
     </row>
@@ -1104,50 +1097,50 @@
         <v>17</v>
       </c>
       <c r="H17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="N17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="O17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="P17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q17" s="19"/>
     </row>
     <row r="18" spans="2:17">
       <c r="C18" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D18" s="18"/>
       <c r="H18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L18" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="M18" t="s">
+        <v>70</v>
+      </c>
+      <c r="N18" t="s">
+        <v>71</v>
+      </c>
+      <c r="O18" t="s">
         <v>72</v>
       </c>
-      <c r="M18" t="s">
-        <v>74</v>
-      </c>
-      <c r="N18" t="s">
-        <v>75</v>
-      </c>
-      <c r="O18" t="s">
-        <v>76</v>
-      </c>
       <c r="P18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="Q18" s="19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:17" ht="31.5">
@@ -1156,25 +1149,25 @@
       </c>
       <c r="D19" s="18"/>
       <c r="H19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M19" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="N19" s="16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="O19" s="16" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="P19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="Q19" s="19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="2:17">
@@ -1183,25 +1176,25 @@
       </c>
       <c r="D20" s="16"/>
       <c r="H20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="M20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="N20" s="16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="O20" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="P20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="Q20" s="19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="2:17">
@@ -1223,7 +1216,7 @@
         <v>9</v>
       </c>
       <c r="H22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L22" t="s">
         <v>8</v>
@@ -1238,7 +1231,7 @@
         <v>9</v>
       </c>
       <c r="P22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="2:17">
@@ -1255,7 +1248,7 @@
         <v>9</v>
       </c>
       <c r="H23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L23" t="s">
         <v>4</v>
@@ -1270,7 +1263,7 @@
         <v>9</v>
       </c>
       <c r="P23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="2:17">
@@ -1287,7 +1280,7 @@
         <v>9</v>
       </c>
       <c r="H24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L24" t="s">
         <v>8</v>
@@ -1302,7 +1295,7 @@
         <v>9</v>
       </c>
       <c r="P24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="2:17" ht="31.5">
@@ -1320,7 +1313,7 @@
         <v>9</v>
       </c>
       <c r="H25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L25" s="16" t="s">
         <v>8</v>
@@ -1335,7 +1328,7 @@
         <v>9</v>
       </c>
       <c r="P25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="2:17">
@@ -1353,7 +1346,7 @@
         <v>9</v>
       </c>
       <c r="H26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L26" s="16" t="s">
         <v>8</v>
@@ -1368,30 +1361,30 @@
         <v>9</v>
       </c>
       <c r="P26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="2:17">
       <c r="B27" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="2:17">
       <c r="C28" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D28" s="16"/>
       <c r="H28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L28" s="20" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="M28" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="N28" s="19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="2:17">
@@ -1414,10 +1407,10 @@
         <v>9</v>
       </c>
       <c r="H30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="M30" t="s">
         <v>9</v>
@@ -1429,7 +1422,7 @@
         <v>9</v>
       </c>
       <c r="P30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="2:17">
@@ -1439,7 +1432,7 @@
     </row>
     <row r="32" spans="2:17">
       <c r="C32" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E32" t="s">
         <v>9</v>
@@ -1451,10 +1444,10 @@
         <v>9</v>
       </c>
       <c r="H32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L32" s="19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="M32" t="s">
         <v>9</v>
@@ -1482,11 +1475,11 @@
         <v>9</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I33" s="3"/>
       <c r="L33" s="17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="M33" s="11" t="s">
         <v>9</v>
@@ -1498,7 +1491,7 @@
         <v>9</v>
       </c>
       <c r="P33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="16.5" thickTop="1">
@@ -1506,27 +1499,17 @@
       <c r="I34" s="2"/>
     </row>
     <row r="35" spans="2:16">
-      <c r="C35" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="C35" s="15"/>
     </row>
     <row r="36" spans="2:16">
-      <c r="C36" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" t="s">
-        <v>43</v>
-      </c>
+      <c r="C36" s="13"/>
       <c r="L36" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="2:16">
-      <c r="D37" t="s">
-        <v>44</v>
-      </c>
       <c r="L37" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename Table 3 as Table 4
....because we're adding variables table.
</commit_message>
<xml_diff>
--- a/manuscript/tables_figures/Table1.xlsx
+++ b/manuscript/tables_figures/Table1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kteixeira/Dropbox (Smithsonian)/GitHub/SCBI-ForestGEO/McGregor_climate-sensitivity-variation/manuscript/tables_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8ACA81-AAC8-3E4E-8667-70210DCFAA39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B006EC-F8B6-7649-A5FC-887C63FE74BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{CE8D29E5-35BD-D341-9E78-19425C1F1F15}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="90">
   <si>
     <t>Prediction</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>(no)</t>
+  </si>
+  <si>
+    <t>Table 4</t>
   </si>
 </sst>
 </file>
@@ -785,7 +788,7 @@
   <dimension ref="B1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -889,6 +892,9 @@
       <c r="G6" s="14" t="s">
         <v>88</v>
       </c>
+      <c r="H6" s="14" t="s">
+        <v>89</v>
+      </c>
       <c r="K6" s="14" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
filled in Table 1
</commit_message>
<xml_diff>
--- a/manuscript/tables_figures/Table1.xlsx
+++ b/manuscript/tables_figures/Table1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kteixeira/Dropbox (Smithsonian)/GitHub/SCBI-ForestGEO/McGregor_climate-sensitivity-variation/manuscript/tables_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0C6906-C160-604E-9CA9-49D50659DDEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53256959-DA6E-F04E-8003-60D2C3E90CE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{CE8D29E5-35BD-D341-9E78-19425C1F1F15}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="93">
   <si>
     <t>Prediction</t>
   </si>
@@ -120,12 +120,6 @@
     <t>H1.2. Drought resistance decreases with crown exposure</t>
   </si>
   <si>
-    <t>1.2a- Crown position alone predicts drought resistance (dominant &lt; co-dominant &lt; intermediate &lt; suppressed)</t>
-  </si>
-  <si>
-    <t>1.2b- After accounting for height, crown position predicts drought resistance (dominant &lt; co-dominant &lt; intermediate &lt; suppressed)</t>
-  </si>
-  <si>
     <t>top_models_dAIC</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t>tested_traits_all &amp; top_models_dAIC</t>
   </si>
   <si>
-    <t>2.3. Negative effect of height persists with inclusion of traits in the statistical model</t>
-  </si>
-  <si>
     <t>H2.3. Size-dependent drought resistance is not driven by functional traits</t>
   </si>
   <si>
@@ -300,7 +291,29 @@
     <t>*this is asking whether height gives better dAIC than DBH</t>
   </si>
   <si>
-    <t>(make SI table)</t>
+    <t>1.2b- After accounting for height, crown position affects drought resistance (dominant trees suffer most)</t>
+  </si>
+  <si>
+    <t>Table S3</t>
+  </si>
+  <si>
+    <t>2.3. Effect of height is negative when traits are included in the statistical model</t>
+  </si>
+  <si>
+    <r>
+      <t>Table S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>#</t>
+    </r>
+  </si>
+  <si>
+    <t>1.2a- Crown position alone affects drought resistance (dominant trees suffer most)</t>
   </si>
 </sst>
 </file>
@@ -373,10 +386,8 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
   <fills count="2">
@@ -472,7 +483,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -484,7 +494,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,18 +812,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F2DC1C-E74B-DD44-87E0-926D1FBF2D78}">
   <dimension ref="B1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="4.6640625" customWidth="1"/>
     <col min="3" max="3" width="75.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="6" max="7" width="8" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
     <col min="12" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.6640625" customWidth="1"/>
     <col min="14" max="14" width="22.6640625" customWidth="1"/>
@@ -825,23 +836,23 @@
     <row r="2" spans="2:16" ht="17" thickTop="1">
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="2:16">
       <c r="B3" s="3"/>
       <c r="C3" s="7"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="2:16" ht="17">
       <c r="B4" s="4"/>
@@ -861,10 +872,10 @@
         <v>1999</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>37</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>1</v>
@@ -879,10 +890,10 @@
         <v>1999</v>
       </c>
       <c r="O4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="P4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:16">
@@ -901,25 +912,25 @@
         <v>4</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="N6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O6" t="s">
         <v>29</v>
@@ -945,31 +956,31 @@
         <v>4</v>
       </c>
       <c r="F8" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="14" t="s">
-        <v>86</v>
-      </c>
       <c r="H8" s="14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="M8" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="18" t="s">
         <v>57</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="O8" t="s">
-        <v>36</v>
-      </c>
-      <c r="P8" s="19" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="17">
@@ -977,275 +988,357 @@
         <v>15</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" t="s">
         <v>85</v>
       </c>
-      <c r="K9" t="s">
-        <v>88</v>
-      </c>
       <c r="L9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="N9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="O9" t="s">
-        <v>50</v>
-      </c>
-      <c r="P9" s="19" t="s">
-        <v>90</v>
+        <v>47</v>
+      </c>
+      <c r="P9" s="18" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="2:16">
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P10" s="19"/>
-    </row>
-    <row r="11" spans="2:16" ht="34">
+      <c r="P10" s="18"/>
+    </row>
+    <row r="11" spans="2:16" ht="17">
       <c r="C11" s="5" t="s">
-        <v>31</v>
+        <v>92</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" t="s">
+        <v>81</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" t="s">
         <v>42</v>
       </c>
-      <c r="L11" t="s">
-        <v>45</v>
-      </c>
       <c r="M11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="N11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="O11" t="s">
         <v>29</v>
       </c>
-      <c r="P11" s="19" t="s">
-        <v>52</v>
+      <c r="P11" s="18" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="36" customHeight="1">
       <c r="C12" s="5" t="s">
-        <v>32</v>
+        <v>88</v>
+      </c>
+      <c r="D12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" t="s">
+        <v>84</v>
       </c>
       <c r="K12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O12" t="s">
-        <v>36</v>
-      </c>
-      <c r="P12" s="19" t="s">
-        <v>53</v>
+        <v>34</v>
+      </c>
+      <c r="P12" s="18" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="2:16">
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P13" s="19" t="s">
-        <v>60</v>
+      <c r="P13" s="18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="34">
       <c r="C14" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" t="s">
+        <v>84</v>
       </c>
       <c r="K14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="N14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="O14" t="s">
-        <v>36</v>
-      </c>
-      <c r="P14" s="19" t="s">
-        <v>60</v>
+        <v>34</v>
+      </c>
+      <c r="P14" s="18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="2:16">
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P15" s="19"/>
+      <c r="P15" s="18"/>
     </row>
     <row r="16" spans="2:16" ht="17">
       <c r="C16" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="N16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O16" t="s">
         <v>29</v>
       </c>
-      <c r="P16" s="19"/>
+      <c r="P16" s="18"/>
     </row>
     <row r="17" spans="2:16" ht="17">
       <c r="C17" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="N17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O17" t="s">
         <v>29</v>
       </c>
-      <c r="P17" s="19"/>
+      <c r="P17" s="18"/>
     </row>
     <row r="18" spans="2:16" ht="17">
       <c r="C18" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+      <c r="E18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>84</v>
       </c>
       <c r="K18" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18" t="s">
+        <v>60</v>
+      </c>
+      <c r="M18" t="s">
         <v>61</v>
       </c>
-      <c r="L18" t="s">
-        <v>63</v>
-      </c>
-      <c r="M18" t="s">
-        <v>64</v>
-      </c>
       <c r="N18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="O18" t="s">
-        <v>36</v>
-      </c>
-      <c r="P18" s="19" t="s">
-        <v>60</v>
+        <v>34</v>
+      </c>
+      <c r="P18" s="18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="34">
       <c r="C19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="18"/>
+      <c r="D19" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" t="s">
+        <v>84</v>
+      </c>
       <c r="K19" s="16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M19" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N19" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P19" s="19" t="s">
-        <v>60</v>
+        <v>34</v>
+      </c>
+      <c r="P19" s="18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="17">
       <c r="C20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="16"/>
+      <c r="D20" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" t="s">
+        <v>84</v>
+      </c>
       <c r="K20" s="16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M20" s="16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="O20" t="s">
-        <v>36</v>
-      </c>
-      <c r="P20" s="19" t="s">
-        <v>60</v>
+        <v>34</v>
+      </c>
+      <c r="P20" s="18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:16">
@@ -1285,7 +1378,7 @@
         <v>9</v>
       </c>
       <c r="O22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="17">
@@ -1320,7 +1413,7 @@
         <v>9</v>
       </c>
       <c r="O23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="2:16" ht="17">
@@ -1355,7 +1448,7 @@
         <v>9</v>
       </c>
       <c r="O24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="2:16" ht="34">
@@ -1390,7 +1483,7 @@
         <v>9</v>
       </c>
       <c r="O25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="17">
@@ -1425,27 +1518,41 @@
         <v>9</v>
       </c>
       <c r="O26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="2:16">
       <c r="B27" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="2:16" ht="17">
       <c r="C28" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" s="16"/>
-      <c r="K28" s="20" t="s">
-        <v>73</v>
+        <v>90</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28" t="s">
+        <v>80</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="K28" s="19" t="s">
+        <v>70</v>
       </c>
       <c r="L28" t="s">
-        <v>69</v>
-      </c>
-      <c r="M28" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
+      </c>
+      <c r="M28" s="18" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="2:16">
@@ -1457,7 +1564,9 @@
       <c r="C30" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="16"/>
+      <c r="D30" s="16" t="s">
+        <v>4</v>
+      </c>
       <c r="E30" t="s">
         <v>9</v>
       </c>
@@ -1467,8 +1576,11 @@
       <c r="G30" t="s">
         <v>9</v>
       </c>
+      <c r="H30" t="s">
+        <v>89</v>
+      </c>
       <c r="K30" s="16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L30" t="s">
         <v>9</v>
@@ -1480,7 +1592,7 @@
         <v>9</v>
       </c>
       <c r="O30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="2:16">
@@ -1490,7 +1602,10 @@
     </row>
     <row r="32" spans="2:16" ht="17">
       <c r="C32" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
       </c>
       <c r="E32" t="s">
         <v>9</v>
@@ -1501,8 +1616,11 @@
       <c r="G32" t="s">
         <v>9</v>
       </c>
-      <c r="K32" s="19" t="s">
-        <v>74</v>
+      <c r="H32" t="s">
+        <v>89</v>
+      </c>
+      <c r="K32" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="L32" t="s">
         <v>9</v>
@@ -1519,7 +1637,9 @@
       <c r="C33" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="17"/>
+      <c r="D33" s="17" t="s">
+        <v>4</v>
+      </c>
       <c r="E33" s="11" t="s">
         <v>9</v>
       </c>
@@ -1529,8 +1649,11 @@
       <c r="G33" s="11" t="s">
         <v>9</v>
       </c>
+      <c r="H33" s="23" t="s">
+        <v>89</v>
+      </c>
       <c r="K33" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L33" s="11" t="s">
         <v>9</v>
@@ -1542,7 +1665,7 @@
         <v>9</v>
       </c>
       <c r="O33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="2:15" ht="17" thickTop="1">
@@ -1554,12 +1677,12 @@
     <row r="36" spans="2:15">
       <c r="C36" s="13"/>
       <c r="K36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="2:15">
       <c r="K37" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
worked on updating display tables with new results
</commit_message>
<xml_diff>
--- a/manuscript/tables_figures/Table1.xlsx
+++ b/manuscript/tables_figures/Table1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kteixeira/Dropbox (Smithsonian)/GitHub/SCBI-ForestGEO/McGregor_climate-sensitivity-variation/manuscript/tables_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53256959-DA6E-F04E-8003-60D2C3E90CE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AF97EE-325E-DE41-AB22-0647CFEA49F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{CE8D29E5-35BD-D341-9E78-19425C1F1F15}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="95">
   <si>
     <t>Prediction</t>
   </si>
@@ -279,9 +279,6 @@
     <t>(no/yes)</t>
   </si>
   <si>
-    <t>Tables 4, S3</t>
-  </si>
-  <si>
     <t>yes, ns ( height dAIC&gt; dbh dAIC, but diff small)</t>
   </si>
   <si>
@@ -292,9 +289,6 @@
   </si>
   <si>
     <t>1.2b- After accounting for height, crown position affects drought resistance (dominant trees suffer most)</t>
-  </si>
-  <si>
-    <t>Table S3</t>
   </si>
   <si>
     <t>2.3. Effect of height is negative when traits are included in the statistical model</t>
@@ -315,12 +309,24 @@
   <si>
     <t>1.2a- Crown position alone affects drought resistance (dominant trees suffer most)</t>
   </si>
+  <si>
+    <t>Table 5</t>
+  </si>
+  <si>
+    <t>usually</t>
+  </si>
+  <si>
+    <t>Tables 4, 5</t>
+  </si>
+  <si>
+    <t>red indicates content that have not been updated since model change</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -389,6 +395,13 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -448,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -485,6 +498,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -494,8 +508,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F2DC1C-E74B-DD44-87E0-926D1FBF2D78}">
-  <dimension ref="B1:P37"/>
+  <dimension ref="B1:P40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -836,23 +850,23 @@
     <row r="2" spans="2:16" ht="17" thickTop="1">
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="2:16">
       <c r="B3" s="3"/>
       <c r="C3" s="7"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="2:16" ht="17">
       <c r="B4" s="4"/>
@@ -940,8 +954,10 @@
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
     </row>
@@ -962,18 +978,18 @@
         <v>83</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="K8" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="K8" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="M8" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="N8" s="24" t="s">
         <v>77</v>
       </c>
       <c r="O8" t="s">
@@ -996,66 +1012,74 @@
       <c r="F9" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="14" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="L9" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="L9" t="s">
-        <v>86</v>
-      </c>
-      <c r="M9" t="s">
-        <v>86</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="M9" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="N9" s="24" t="s">
         <v>48</v>
       </c>
       <c r="O9" t="s">
         <v>47</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="2:16">
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
       <c r="P10" s="18"/>
     </row>
     <row r="11" spans="2:16" ht="17">
       <c r="C11" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F11" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F11" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="14" t="s">
         <v>81</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="24" t="s">
         <v>43</v>
       </c>
       <c r="O11" t="s">
@@ -1067,33 +1091,33 @@
     </row>
     <row r="12" spans="2:16" ht="36" customHeight="1">
       <c r="C12" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="E12" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="H12" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="F12" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="K12" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="24" t="s">
         <v>76</v>
       </c>
       <c r="O12" t="s">
@@ -1107,6 +1131,14 @@
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
       <c r="P13" s="18" t="s">
         <v>57</v>
       </c>
@@ -1115,31 +1147,31 @@
       <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="D14" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="G14" t="s">
+      <c r="E14" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="H14" t="s">
-        <v>84</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="F14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="K14" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="24" t="s">
         <v>55</v>
       </c>
       <c r="O14" t="s">
@@ -1153,37 +1185,45 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
       <c r="P15" s="18"/>
     </row>
     <row r="16" spans="2:16" ht="17">
       <c r="C16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D16" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="24" t="s">
         <v>80</v>
       </c>
       <c r="H16" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16" s="24" t="s">
         <v>45</v>
       </c>
       <c r="O16" t="s">
@@ -1195,31 +1235,31 @@
       <c r="C17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D17" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="D17" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="24" t="s">
         <v>80</v>
       </c>
       <c r="H17" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="24" t="s">
         <v>45</v>
       </c>
       <c r="O17" t="s">
@@ -1231,31 +1271,31 @@
       <c r="C18" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="D18" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H18" t="s">
-        <v>84</v>
-      </c>
-      <c r="K18" s="16" t="s">
+      <c r="H18" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="K18" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" s="24" t="s">
         <v>62</v>
       </c>
       <c r="O18" t="s">
@@ -1269,31 +1309,31 @@
       <c r="C19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F19" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" t="s">
-        <v>80</v>
-      </c>
-      <c r="H19" t="s">
-        <v>84</v>
-      </c>
-      <c r="K19" s="16" t="s">
+      <c r="F19" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="K19" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="L19" s="16" t="s">
+      <c r="L19" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="M19" s="16" t="s">
+      <c r="M19" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="N19" s="16" t="s">
+      <c r="N19" s="24" t="s">
         <v>74</v>
       </c>
       <c r="O19" t="s">
@@ -1307,31 +1347,31 @@
       <c r="C20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E20" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="E20" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G20" t="s">
-        <v>80</v>
-      </c>
-      <c r="H20" t="s">
-        <v>84</v>
-      </c>
-      <c r="K20" s="16" t="s">
+      <c r="G20" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="K20" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="M20" s="16" t="s">
+      <c r="M20" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N20" s="24" t="s">
         <v>75</v>
       </c>
       <c r="O20" t="s">
@@ -1362,8 +1402,8 @@
       <c r="G22" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="24" t="s">
-        <v>91</v>
+      <c r="H22" s="20" t="s">
+        <v>89</v>
       </c>
       <c r="K22" t="s">
         <v>8</v>
@@ -1397,8 +1437,8 @@
       <c r="G23" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="24" t="s">
-        <v>91</v>
+      <c r="H23" s="20" t="s">
+        <v>89</v>
       </c>
       <c r="K23" t="s">
         <v>4</v>
@@ -1432,8 +1472,8 @@
       <c r="G24" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="24" t="s">
-        <v>91</v>
+      <c r="H24" s="20" t="s">
+        <v>89</v>
       </c>
       <c r="K24" t="s">
         <v>8</v>
@@ -1467,8 +1507,8 @@
       <c r="G25" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="24" t="s">
-        <v>91</v>
+      <c r="H25" s="20" t="s">
+        <v>89</v>
       </c>
       <c r="K25" s="16" t="s">
         <v>8</v>
@@ -1502,8 +1542,8 @@
       <c r="G26" t="s">
         <v>9</v>
       </c>
-      <c r="H26" s="24" t="s">
-        <v>91</v>
+      <c r="H26" s="20" t="s">
+        <v>89</v>
       </c>
       <c r="K26" s="16" t="s">
         <v>8</v>
@@ -1528,7 +1568,7 @@
     </row>
     <row r="28" spans="2:16" ht="17">
       <c r="C28" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D28" s="16" t="s">
         <v>4</v>
@@ -1543,7 +1583,7 @@
         <v>80</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="K28" s="19" t="s">
         <v>70</v>
@@ -1565,7 +1605,7 @@
         <v>28</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E30" t="s">
         <v>9</v>
@@ -1577,7 +1617,7 @@
         <v>9</v>
       </c>
       <c r="H30" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="K30" s="16" t="s">
         <v>68</v>
@@ -1605,7 +1645,7 @@
         <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="E32" t="s">
         <v>9</v>
@@ -1616,8 +1656,8 @@
       <c r="G32" t="s">
         <v>9</v>
       </c>
-      <c r="H32" t="s">
-        <v>89</v>
+      <c r="H32" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="K32" s="18" t="s">
         <v>71</v>
@@ -1649,10 +1689,10 @@
       <c r="G33" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="K33" s="17" t="s">
+      <c r="H33" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="K33" s="25" t="s">
         <v>69</v>
       </c>
       <c r="L33" s="11" t="s">
@@ -1683,6 +1723,11 @@
     <row r="37" spans="2:15">
       <c r="K37" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15">
+      <c r="K40" s="24" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated tables 1 and 4 with new results, formatted table 5, made some edits to draft
</commit_message>
<xml_diff>
--- a/manuscript/tables_figures/Table1.xlsx
+++ b/manuscript/tables_figures/Table1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kteixeira/Dropbox (Smithsonian)/GitHub/SCBI-ForestGEO/McGregor_climate-sensitivity-variation/manuscript/tables_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AF97EE-325E-DE41-AB22-0647CFEA49F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC61986-D91D-A545-A1EA-4E2EE71773FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{CE8D29E5-35BD-D341-9E78-19425C1F1F15}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="97">
   <si>
     <t>Prediction</t>
   </si>
@@ -195,9 +195,6 @@
     <t>no (tta, ns); no (tmd* interaction does not appear in top models)</t>
   </si>
   <si>
-    <t xml:space="preserve">2.1c - more diffuse porous species correlates negatively to drought resistance </t>
-  </si>
-  <si>
     <t>*for all within the tmd table, the covariate is included within the set of other covariates, so the effect of this specific covariate by itself is only interpreted from the coefficients, not the dAIC (all of these models are &lt;2 anyways)</t>
   </si>
   <si>
@@ -244,9 +241,6 @@
   </si>
   <si>
     <t>yes (tta, ns); no (tmd* interaction does not appear in top models)</t>
-  </si>
-  <si>
-    <t>yes (tta, ns); yes (tmd*, TLP appears in 1 of 3 top models and is yes for that one)</t>
   </si>
   <si>
     <t>yes (tta, ns);  yes (tmd*, PLA appears in 4 of 9 top models, and is yes for those)</t>
@@ -320,6 +314,18 @@
   </si>
   <si>
     <t>red indicates content that have not been updated since model change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1c - diffuse porous species have lower drought resistance </t>
+  </si>
+  <si>
+    <t>yes (tta, ns);  yes (tmd*, TLP appears in some top models and is yes for all of them)</t>
+  </si>
+  <si>
+    <t>(yes/no)</t>
+  </si>
+  <si>
+    <t>yes (tta, ns); yes (tmd*, TLP appears in 2 top models and is no for both)</t>
   </si>
 </sst>
 </file>
@@ -826,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F2DC1C-E74B-DD44-87E0-926D1FBF2D78}">
   <dimension ref="B1:P40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -835,7 +841,7 @@
     <col min="2" max="2" width="4.6640625" customWidth="1"/>
     <col min="3" max="3" width="75.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" customWidth="1"/>
     <col min="6" max="7" width="8" customWidth="1"/>
     <col min="11" max="11" width="19.6640625" customWidth="1"/>
     <col min="12" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
@@ -876,8 +882,8 @@
       <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>3</v>
+      <c r="E4" s="9">
+        <v>1966</v>
       </c>
       <c r="F4" s="9">
         <v>1977</v>
@@ -926,13 +932,13 @@
         <v>4</v>
       </c>
       <c r="F6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>80</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>82</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>44</v>
@@ -972,31 +978,31 @@
         <v>4</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L8" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M8" s="24" t="s">
         <v>54</v>
       </c>
       <c r="N8" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O8" t="s">
         <v>34</v>
       </c>
       <c r="P8" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="17">
@@ -1004,28 +1010,28 @@
         <v>15</v>
       </c>
       <c r="D9" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="14" t="s">
+      <c r="K9" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="24" t="s">
-        <v>84</v>
-      </c>
       <c r="L9" s="24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N9" s="24" t="s">
         <v>48</v>
@@ -1034,7 +1040,7 @@
         <v>47</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="2:16">
@@ -1053,22 +1059,22 @@
     </row>
     <row r="11" spans="2:16" ht="17">
       <c r="C11" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="14" t="s">
         <v>80</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>82</v>
       </c>
       <c r="K11" s="24" t="s">
         <v>39</v>
@@ -1091,22 +1097,22 @@
     </row>
     <row r="12" spans="2:16" ht="36" customHeight="1">
       <c r="C12" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K12" s="24" t="s">
         <v>52</v>
@@ -1118,7 +1124,7 @@
         <v>53</v>
       </c>
       <c r="N12" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O12" t="s">
         <v>34</v>
@@ -1140,7 +1146,7 @@
       <c r="M13" s="24"/>
       <c r="N13" s="24"/>
       <c r="P13" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="34">
@@ -1148,25 +1154,25 @@
         <v>33</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K14" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L14" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M14" s="24" t="s">
         <v>55</v>
@@ -1178,7 +1184,7 @@
         <v>34</v>
       </c>
       <c r="P14" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="2:16">
@@ -1199,20 +1205,20 @@
       <c r="C16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" s="14" t="s">
         <v>80</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>82</v>
       </c>
       <c r="K16" s="24" t="s">
         <v>45</v>
@@ -1235,20 +1241,20 @@
       <c r="C17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="14" t="s">
         <v>80</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>82</v>
       </c>
       <c r="K17" s="24" t="s">
         <v>45</v>
@@ -1269,116 +1275,116 @@
     </row>
     <row r="18" spans="2:16" ht="17">
       <c r="C18" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="G18" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="14" t="s">
         <v>4</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K18" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L18" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="M18" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="M18" s="24" t="s">
+      <c r="N18" s="24" t="s">
         <v>61</v>
-      </c>
-      <c r="N18" s="24" t="s">
-        <v>62</v>
       </c>
       <c r="O18" t="s">
         <v>34</v>
       </c>
       <c r="P18" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="34">
       <c r="C19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>80</v>
+      <c r="F19" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K19" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L19" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="L19" s="24" t="s">
-        <v>64</v>
-      </c>
       <c r="M19" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N19" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="O19" t="s">
         <v>34</v>
       </c>
       <c r="P19" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="17">
       <c r="C20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>80</v>
+      <c r="D20" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="K20" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="L20" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="M20" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="N20" s="24" t="s">
         <v>73</v>
-      </c>
-      <c r="M20" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="N20" s="24" t="s">
-        <v>75</v>
       </c>
       <c r="O20" t="s">
         <v>34</v>
       </c>
       <c r="P20" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="2:16">
@@ -1403,7 +1409,7 @@
         <v>9</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K22" t="s">
         <v>8</v>
@@ -1438,7 +1444,7 @@
         <v>9</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K23" t="s">
         <v>4</v>
@@ -1473,7 +1479,7 @@
         <v>9</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K24" t="s">
         <v>8</v>
@@ -1508,7 +1514,7 @@
         <v>9</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K25" s="16" t="s">
         <v>8</v>
@@ -1543,7 +1549,7 @@
         <v>9</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K26" s="16" t="s">
         <v>8</v>
@@ -1568,7 +1574,7 @@
     </row>
     <row r="28" spans="2:16" ht="17">
       <c r="C28" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D28" s="16" t="s">
         <v>4</v>
@@ -1577,22 +1583,22 @@
         <v>4</v>
       </c>
       <c r="F28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L28" t="s">
+        <v>65</v>
+      </c>
+      <c r="M28" s="18" t="s">
         <v>66</v>
-      </c>
-      <c r="M28" s="18" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="29" spans="2:16">
@@ -1617,10 +1623,10 @@
         <v>9</v>
       </c>
       <c r="H30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L30" t="s">
         <v>9</v>
@@ -1645,7 +1651,7 @@
         <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E32" t="s">
         <v>9</v>
@@ -1657,10 +1663,10 @@
         <v>9</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K32" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L32" t="s">
         <v>9</v>
@@ -1690,10 +1696,10 @@
         <v>9</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K33" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L33" s="11" t="s">
         <v>9</v>
@@ -1727,7 +1733,7 @@
     </row>
     <row r="40" spans="2:15">
       <c r="K40" s="24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>